<commit_message>
Change native status from Invasive to Introduced to match USDA Plants terminology
</commit_message>
<xml_diff>
--- a/data/raw/seed-mix.xlsx
+++ b/data/raw/seed-mix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F6C53ED-9000-4185-881E-213EBA48EEC7}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{6B8EBC92-27E1-4B6B-95EC-F86A8BD3054F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{405F4FFE-791A-4C0C-A1D8-284F8E4351B4}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="21624" windowHeight="11112" xr2:uid="{0CAD531B-17AC-4CC0-8784-EF62A45F9D76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="236">
   <si>
     <t>Family</t>
   </si>
@@ -741,6 +741,9 @@
   </si>
   <si>
     <t>Region</t>
+  </si>
+  <si>
+    <t>Native</t>
   </si>
 </sst>
 </file>
@@ -793,6 +796,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1092,11 +1099,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ED48DE-F67E-409C-BADB-8346B0730F99}">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1109,7 +1116,7 @@
     <col min="6" max="6" width="31.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>234</v>
       </c>
@@ -1134,8 +1141,11 @@
       <c r="H1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>230</v>
       </c>
@@ -1160,8 +1170,11 @@
       <c r="H2">
         <v>16.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>230</v>
       </c>
@@ -1186,8 +1199,11 @@
       <c r="H3">
         <v>17.72</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>230</v>
       </c>
@@ -1212,8 +1228,11 @@
       <c r="H4">
         <v>17.97</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -1238,8 +1257,11 @@
       <c r="H5">
         <v>18.63</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>230</v>
       </c>
@@ -1264,8 +1286,11 @@
       <c r="H6">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>230</v>
       </c>
@@ -1290,8 +1315,11 @@
       <c r="H7">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>230</v>
       </c>
@@ -1316,8 +1344,11 @@
       <c r="H8">
         <v>19.899999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>230</v>
       </c>
@@ -1342,8 +1373,11 @@
       <c r="H9">
         <v>19.899999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>230</v>
       </c>
@@ -1368,8 +1402,11 @@
       <c r="H10">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>230</v>
       </c>
@@ -1394,8 +1431,11 @@
       <c r="H11">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>230</v>
       </c>
@@ -1420,8 +1460,11 @@
       <c r="H12">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>230</v>
       </c>
@@ -1446,8 +1489,11 @@
       <c r="H13">
         <v>21.84</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>230</v>
       </c>
@@ -1472,8 +1518,11 @@
       <c r="H14">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -1498,8 +1547,11 @@
       <c r="H15">
         <v>23.15</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>230</v>
       </c>
@@ -1524,8 +1576,11 @@
       <c r="H16">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>230</v>
       </c>
@@ -1550,8 +1605,11 @@
       <c r="H17">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>230</v>
       </c>
@@ -1576,8 +1634,11 @@
       <c r="H18">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>230</v>
       </c>
@@ -1602,8 +1663,11 @@
       <c r="H19">
         <v>15.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>230</v>
       </c>
@@ -1628,8 +1692,11 @@
       <c r="H20">
         <v>15.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>230</v>
       </c>
@@ -1654,8 +1721,11 @@
       <c r="H21">
         <v>15.95</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>230</v>
       </c>
@@ -1680,8 +1750,11 @@
       <c r="H22">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>71</v>
       </c>
@@ -1706,8 +1779,11 @@
       <c r="H23">
         <v>11.4</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>71</v>
       </c>
@@ -1732,8 +1808,11 @@
       <c r="H24">
         <v>11.7</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -1758,8 +1837,11 @@
       <c r="H25">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1784,8 +1866,11 @@
       <c r="H26">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -1810,8 +1895,11 @@
       <c r="H27">
         <v>12.7</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -1836,8 +1924,11 @@
       <c r="H28">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -1859,8 +1950,11 @@
       <c r="G29">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1885,8 +1979,11 @@
       <c r="H30">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -1911,8 +2008,11 @@
       <c r="H31">
         <v>13.7</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1937,8 +2037,11 @@
       <c r="H32">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -1963,8 +2066,11 @@
       <c r="H33">
         <v>15.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -1989,8 +2095,11 @@
       <c r="H34">
         <v>15.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -2015,8 +2124,11 @@
       <c r="H35">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -2041,8 +2153,11 @@
       <c r="H36">
         <v>15.9</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>71</v>
       </c>
@@ -2067,8 +2182,11 @@
       <c r="H37">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -2093,8 +2211,11 @@
       <c r="H38">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -2119,8 +2240,11 @@
       <c r="H39">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -2145,8 +2269,11 @@
       <c r="H40">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -2171,8 +2298,11 @@
       <c r="H41">
         <v>17.100000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -2197,8 +2327,11 @@
       <c r="H42">
         <v>17.399999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>71</v>
       </c>
@@ -2223,8 +2356,11 @@
       <c r="H43">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -2246,8 +2382,11 @@
       <c r="G44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>71</v>
       </c>
@@ -2272,8 +2411,11 @@
       <c r="H45">
         <v>18.3</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>71</v>
       </c>
@@ -2298,8 +2440,11 @@
       <c r="H46">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -2324,8 +2469,11 @@
       <c r="H47">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I47" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>71</v>
       </c>
@@ -2350,8 +2498,11 @@
       <c r="H48">
         <v>21.1</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I48" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>71</v>
       </c>
@@ -2376,8 +2527,11 @@
       <c r="H49">
         <v>21.4</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I49" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>71</v>
       </c>
@@ -2402,8 +2556,11 @@
       <c r="H50">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>71</v>
       </c>
@@ -2428,8 +2585,11 @@
       <c r="H51">
         <v>21.7</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I51" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -2454,8 +2614,11 @@
       <c r="H52">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I52" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>231</v>
       </c>
@@ -2480,8 +2643,11 @@
       <c r="H53">
         <v>17.97</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>231</v>
       </c>
@@ -2506,8 +2672,11 @@
       <c r="H54">
         <v>20.25</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>231</v>
       </c>
@@ -2532,8 +2701,11 @@
       <c r="H55">
         <v>19.86</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I55" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>231</v>
       </c>
@@ -2558,8 +2730,11 @@
       <c r="H56">
         <v>21.84</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>231</v>
       </c>
@@ -2584,8 +2759,11 @@
       <c r="H57">
         <v>21.94</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I57" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>231</v>
       </c>
@@ -2610,8 +2788,11 @@
       <c r="H58">
         <v>23.31</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>231</v>
       </c>
@@ -2636,8 +2817,11 @@
       <c r="H59">
         <v>20.25</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I59" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>231</v>
       </c>
@@ -2659,8 +2843,11 @@
       <c r="G60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I60" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>231</v>
       </c>
@@ -2685,8 +2872,11 @@
       <c r="H61">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I61" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>231</v>
       </c>
@@ -2711,8 +2901,11 @@
       <c r="H62">
         <v>22.96</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I62" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>231</v>
       </c>
@@ -2737,8 +2930,11 @@
       <c r="H63">
         <v>23.18</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I63" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>231</v>
       </c>
@@ -2763,8 +2959,11 @@
       <c r="H64">
         <v>23.33</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I64" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>231</v>
       </c>
@@ -2789,8 +2988,11 @@
       <c r="H65">
         <v>23.38</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I65" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>231</v>
       </c>
@@ -2815,8 +3017,11 @@
       <c r="H66">
         <v>23.38</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I66" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>231</v>
       </c>
@@ -2841,8 +3046,11 @@
       <c r="H67">
         <v>23.52</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I67" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>231</v>
       </c>
@@ -2864,8 +3072,11 @@
       <c r="G68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I68" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>232</v>
       </c>
@@ -2890,8 +3101,11 @@
       <c r="H69">
         <v>13.7</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I69" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>232</v>
       </c>
@@ -2916,8 +3130,11 @@
       <c r="H70">
         <v>16.25</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I70" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>232</v>
       </c>
@@ -2942,8 +3159,11 @@
       <c r="H71">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I71" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>232</v>
       </c>
@@ -2968,8 +3188,11 @@
       <c r="H72">
         <v>17.97</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I72" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>232</v>
       </c>
@@ -2994,8 +3217,11 @@
       <c r="H73">
         <v>18.63</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I73" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>232</v>
       </c>
@@ -3020,8 +3246,11 @@
       <c r="H74">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I74" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>232</v>
       </c>
@@ -3043,8 +3272,11 @@
       <c r="G75">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I75" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>232</v>
       </c>
@@ -3069,8 +3301,11 @@
       <c r="H76">
         <v>15.97</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I76" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>232</v>
       </c>
@@ -3095,8 +3330,11 @@
       <c r="H77">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I77" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>232</v>
       </c>
@@ -3121,8 +3359,11 @@
       <c r="H78">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I78" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>232</v>
       </c>
@@ -3147,8 +3388,11 @@
       <c r="H79">
         <v>21.1</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I79" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>232</v>
       </c>
@@ -3173,8 +3417,11 @@
       <c r="H80">
         <v>21.7</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I80" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>232</v>
       </c>
@@ -3199,8 +3446,11 @@
       <c r="H81">
         <v>21.84</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I81" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>232</v>
       </c>
@@ -3225,8 +3475,11 @@
       <c r="H82">
         <v>23.15</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I82" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>233</v>
       </c>
@@ -3251,8 +3504,11 @@
       <c r="H83">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I83" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>233</v>
       </c>
@@ -3277,8 +3533,11 @@
       <c r="H84">
         <v>21.84</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I84" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>233</v>
       </c>
@@ -3303,8 +3562,11 @@
       <c r="H85">
         <v>22.96</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I85" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>233</v>
       </c>
@@ -3329,8 +3591,11 @@
       <c r="H86">
         <v>22.89</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I86" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>233</v>
       </c>
@@ -3355,8 +3620,11 @@
       <c r="H87">
         <v>22.87</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I87" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>233</v>
       </c>
@@ -3381,8 +3649,11 @@
       <c r="H88">
         <v>21.75</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I88" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>233</v>
       </c>
@@ -3407,8 +3678,11 @@
       <c r="H89">
         <v>20.86</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I89" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>233</v>
       </c>
@@ -3433,8 +3707,11 @@
       <c r="H90">
         <v>21.66</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I90" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>233</v>
       </c>
@@ -3459,8 +3736,11 @@
       <c r="H91">
         <v>23.46</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I91" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>233</v>
       </c>
@@ -3485,8 +3765,11 @@
       <c r="H92">
         <v>23.15</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I92" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>233</v>
       </c>
@@ -3511,8 +3794,11 @@
       <c r="H93">
         <v>23.38</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I93" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>233</v>
       </c>
@@ -3537,8 +3823,11 @@
       <c r="H94">
         <v>23.97</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I94" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>233</v>
       </c>
@@ -3563,8 +3852,11 @@
       <c r="H95">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I95" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>233</v>
       </c>
@@ -3589,8 +3881,11 @@
       <c r="H96">
         <v>23.83</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I96" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>233</v>
       </c>
@@ -3615,8 +3910,11 @@
       <c r="H97">
         <v>24.88</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I97" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>233</v>
       </c>
@@ -3640,6 +3938,9 @@
       </c>
       <c r="H98">
         <v>24.2</v>
+      </c>
+      <c r="I98" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>